<commit_message>
all finished test for API functions, add logIn, logOut, isLogIn API to documents/api명세서.
</commit_message>
<xml_diff>
--- a/documents/API 명세서.xlsx
+++ b/documents/API 명세서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\TJSManager_main\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF51F69B-DDB0-4F89-BCC8-1759A59690A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF1B44-8729-4685-85CC-B80736308A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="249">
   <si>
     <t>시스템</t>
   </si>
@@ -158,9 +158,6 @@
     <t>모든 입고 신청서 조회</t>
   </si>
   <si>
-    <t>req_num: int</t>
-  </si>
-  <si>
     <t>한 입고 신청서 조회</t>
   </si>
   <si>
@@ -170,12 +167,6 @@
     <t>입고 신청서 삭제</t>
   </si>
   <si>
-    <t>모든 최종 입고 신청 이력 조회</t>
-  </si>
-  <si>
-    <t>한 최종 입고 신청 이력 조회</t>
-  </si>
-  <si>
     <t>/item/stock</t>
   </si>
   <si>
@@ -411,26 +402,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/item/req_in_warehouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/item/req_in_warehouse/{report_num}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getAllReqInWarehouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/item/req_in_warehouse/{req_num}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getOneReqInWarehouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>/item/in_warehouse_report/{report_num}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -471,10 +442,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>모든 물품별 구매자 기록</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>getAllSalesConsumer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -511,10 +478,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>한 물품별 구매자 기록</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>getOneSalesConsumer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -672,10 +635,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>salesNum: Long(1)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>consumerGender: String("m"/"f")</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -736,10 +695,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>입고 신청 최종 승인 | 최종 입고 신청 이력 생성</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>inCnt: int(3 등)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -802,10 +757,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>물품별 구매자 기록 생성</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>판매 이력 기록 생성</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -879,6 +830,90 @@
   </si>
   <si>
     <t>storeTelNum: String(지점 전화번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매자 기록 생성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 구매자 기록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 구매자 기록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매자 기록 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateSalesConsumer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매 이력 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateSalesRecord</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HRM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employeeLogin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemNum: Long(물품 번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>empNum: String(직원 번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>empPassword: String(직원 비밀번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employee/log_out</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employee/log_in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employeeLogIOut</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employee/is_log_in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 여부 확인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employeeIsLogIn</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -968,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -980,6 +1015,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1294,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1309,15 +1350,15 @@
     <col min="5" max="5" width="29.19921875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.19921875" style="4" customWidth="1"/>
     <col min="7" max="7" width="47.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.8984375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.59765625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.69921875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.19921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.19921875" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="34.19921875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="41.8984375" bestFit="1" customWidth="1"/>
@@ -1345,10 +1386,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>5</v>
@@ -1364,152 +1405,93 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>106</v>
+    <row r="2" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="I2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" t="s">
-        <v>173</v>
-      </c>
-      <c r="K2" t="s">
-        <v>174</v>
-      </c>
-      <c r="L2" t="s">
-        <v>175</v>
-      </c>
-      <c r="N2"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="N3"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U3" t="s">
-        <v>14</v>
-      </c>
-      <c r="V3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W3" t="s">
-        <v>16</v>
-      </c>
-      <c r="X3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>23</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
+      <c r="A4" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="N4"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4" t="s">
-        <v>12</v>
-      </c>
-      <c r="T4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" t="s">
-        <v>14</v>
-      </c>
-      <c r="V4" t="s">
-        <v>15</v>
-      </c>
-      <c r="W4" t="s">
-        <v>16</v>
-      </c>
-      <c r="X4" t="s">
-        <v>22</v>
+        <v>247</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.4">
@@ -1520,62 +1502,88 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="J5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="K5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="L5" t="s">
-        <v>175</v>
-      </c>
-      <c r="N5"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>28</v>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="O6" s="6"/>
+        <v>208</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
@@ -1585,693 +1593,692 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>176</v>
+        <v>106</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H7" t="s">
-        <v>177</v>
-      </c>
-      <c r="I7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J7" t="s">
-        <v>179</v>
-      </c>
-      <c r="K7" t="s">
-        <v>180</v>
-      </c>
-      <c r="N7"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="4"/>
+        <v>208</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" t="s">
+        <v>21</v>
+      </c>
+      <c r="S7" t="s">
+        <v>12</v>
+      </c>
+      <c r="T7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" t="s">
+        <v>15</v>
+      </c>
+      <c r="W7" t="s">
+        <v>16</v>
+      </c>
+      <c r="X7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>26</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>184</v>
+        <v>27</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="N8"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" t="s">
-        <v>136</v>
+        <v>208</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K8" t="s">
+        <v>164</v>
+      </c>
+      <c r="L8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>187</v>
+        <v>29</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="N9"/>
+        <v>208</v>
+      </c>
       <c r="O9" s="6"/>
-      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" t="s">
         <v>167</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="N10"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="4"/>
+      <c r="I10" t="s">
+        <v>168</v>
+      </c>
+      <c r="J10" t="s">
+        <v>169</v>
+      </c>
+      <c r="K10" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>229</v>
+        <v>174</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N11"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="4"/>
+        <v>208</v>
+      </c>
+      <c r="H11"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>232</v>
+        <v>176</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>231</v>
+        <v>177</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>227</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="H12"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C13" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="K13" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N14" s="4"/>
+        <v>214</v>
+      </c>
+      <c r="H14"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>217</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="J15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L15" t="s">
-        <v>192</v>
-      </c>
-      <c r="N15"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="4"/>
+        <v>219</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H15"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="4"/>
+      <c r="P15"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H17"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J18" t="s">
+        <v>180</v>
+      </c>
+      <c r="K18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="P19" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>131</v>
+      </c>
+      <c r="R19" t="s">
         <v>132</v>
       </c>
-      <c r="B16" t="s">
+      <c r="S19" t="s">
         <v>133</v>
       </c>
-      <c r="C16" t="s">
+      <c r="T19" t="s">
+        <v>134</v>
+      </c>
+      <c r="U19" t="s">
         <v>135</v>
       </c>
-      <c r="D16" t="s">
+      <c r="V19" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="6" t="s">
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
         <v>137</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="D20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="N16"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="4" t="s">
+      <c r="G20" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="Q20" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="R20" t="s">
+        <v>132</v>
+      </c>
+      <c r="S20" t="s">
+        <v>133</v>
+      </c>
+      <c r="T20" t="s">
+        <v>134</v>
+      </c>
+      <c r="U20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I21" t="s">
+        <v>179</v>
+      </c>
+      <c r="J21" t="s">
+        <v>180</v>
+      </c>
+      <c r="K21" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q21" s="4"/>
+    </row>
+    <row r="22" spans="1:29" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="Q22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="F23" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="R16" t="s">
+      <c r="G23" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="R23" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="S23" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T23" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U23" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V23" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W23" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="X23" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="F24" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="N17"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="R17" t="s">
-        <v>141</v>
-      </c>
-      <c r="S17" t="s">
-        <v>142</v>
-      </c>
-      <c r="T17" t="s">
-        <v>143</v>
-      </c>
-      <c r="U17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="O18" s="7"/>
-      <c r="Q18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="R19" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="S19" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="T19" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="U19" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="V19" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="W19" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="X19" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20" s="6"/>
-      <c r="Q20" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="R20" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="S20" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="T20" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="U20" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="V20" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="W20" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="X20" s="8"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J21" t="s">
-        <v>200</v>
-      </c>
-      <c r="K21" t="s">
-        <v>201</v>
-      </c>
-      <c r="L21" t="s">
-        <v>202</v>
-      </c>
-      <c r="M21" t="s">
-        <v>203</v>
-      </c>
-      <c r="N21"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" s="4"/>
-      <c r="N22"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>20</v>
-      </c>
-      <c r="R22" t="s">
-        <v>116</v>
-      </c>
-      <c r="S22" t="s">
-        <v>34</v>
-      </c>
-      <c r="T22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U22" t="s">
-        <v>39</v>
-      </c>
-      <c r="V22" t="s">
-        <v>22</v>
-      </c>
-      <c r="W22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="N23"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" t="s">
-        <v>20</v>
-      </c>
-      <c r="R23" t="s">
-        <v>116</v>
-      </c>
-      <c r="S23" t="s">
-        <v>34</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U23" t="s">
-        <v>39</v>
-      </c>
-      <c r="V23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J24" t="s">
-        <v>200</v>
-      </c>
-      <c r="K24" t="s">
-        <v>201</v>
-      </c>
-      <c r="L24" t="s">
-        <v>202</v>
-      </c>
-      <c r="M24" t="s">
-        <v>203</v>
-      </c>
+      <c r="G24" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
       <c r="N24"/>
       <c r="O24" s="6"/>
-      <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
+      <c r="Q24" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="S24" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="T24" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="U24" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="V24" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="W24" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="X24" s="8"/>
+    </row>
+    <row r="25" spans="1:29" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.4">
+        <v>233</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25" s="6"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2279,19 +2286,37 @@
         <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J26" t="s">
+        <v>189</v>
+      </c>
+      <c r="K26" t="s">
+        <v>190</v>
+      </c>
+      <c r="L26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2299,43 +2324,46 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="O27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="P27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>20</v>
       </c>
-      <c r="Q27" t="s">
-        <v>41</v>
-      </c>
       <c r="R27" t="s">
+        <v>113</v>
+      </c>
+      <c r="S27" t="s">
         <v>34</v>
       </c>
-      <c r="S27" s="3" t="s">
+      <c r="T27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>39</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>22</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2343,37 +2371,40 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="P28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q28" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" t="s">
-        <v>41</v>
-      </c>
       <c r="R28" t="s">
+        <v>113</v>
+      </c>
+      <c r="S28" t="s">
         <v>34</v>
       </c>
-      <c r="S28" s="3" t="s">
+      <c r="T28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>39</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2381,37 +2412,40 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" t="s">
-        <v>205</v>
-      </c>
-      <c r="H29" t="s">
-        <v>206</v>
-      </c>
-      <c r="I29" t="s">
-        <v>207</v>
+        <v>42</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="J29" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="K29" t="s">
-        <v>209</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.4">
+        <v>190</v>
+      </c>
+      <c r="L29" t="s">
+        <v>191</v>
+      </c>
+      <c r="M29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2419,55 +2453,26 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="O30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P30" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R30" t="s">
-        <v>34</v>
-      </c>
-      <c r="S30" t="s">
-        <v>49</v>
-      </c>
-      <c r="T30" t="s">
-        <v>50</v>
-      </c>
-      <c r="U30" t="s">
-        <v>51</v>
-      </c>
-      <c r="V30" t="s">
-        <v>52</v>
-      </c>
-      <c r="W30" t="s">
-        <v>53</v>
-      </c>
-      <c r="X30" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="4"/>
+      <c r="P30"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2475,88 +2480,105 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>210</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="J31" t="s">
+        <v>193</v>
+      </c>
+      <c r="K31" t="s">
+        <v>194</v>
+      </c>
+      <c r="L31" t="s">
+        <v>195</v>
+      </c>
+      <c r="M31" t="s">
+        <v>196</v>
+      </c>
+      <c r="N31" t="s">
+        <v>197</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="P31" t="s">
+      <c r="E32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q32" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="3" t="s">
+      <c r="R32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S32" t="s">
         <v>34</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T32" t="s">
+        <v>46</v>
+      </c>
+      <c r="U32" t="s">
+        <v>47</v>
+      </c>
+      <c r="V32" t="s">
+        <v>48</v>
+      </c>
+      <c r="W32" t="s">
         <v>49</v>
       </c>
-      <c r="T31" t="s">
+      <c r="X32" t="s">
         <v>50</v>
       </c>
-      <c r="U31" t="s">
+      <c r="Y32" t="s">
         <v>51</v>
       </c>
-      <c r="V31" t="s">
-        <v>52</v>
-      </c>
-      <c r="W31" t="s">
-        <v>53</v>
-      </c>
-      <c r="X31" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA31" t="s">
+      <c r="AB32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>132</v>
-      </c>
-      <c r="B32" t="s">
-        <v>160</v>
-      </c>
-      <c r="C32" t="s">
-        <v>210</v>
-      </c>
-      <c r="D32" t="s">
-        <v>161</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="G32" t="s">
-        <v>205</v>
-      </c>
-      <c r="H32" t="s">
-        <v>206</v>
-      </c>
-      <c r="I32" t="s">
-        <v>207</v>
-      </c>
-      <c r="J32" t="s">
-        <v>208</v>
-      </c>
-      <c r="K32" t="s">
-        <v>209</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q32" s="4"/>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="AC32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2564,85 +2586,94 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>17</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>213</v>
+        <v>53</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G33" t="s">
-        <v>214</v>
-      </c>
-      <c r="H33" t="s">
-        <v>215</v>
-      </c>
-      <c r="I33" t="s">
-        <v>216</v>
-      </c>
-      <c r="J33" t="s">
-        <v>217</v>
-      </c>
-      <c r="K33" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q33" s="4"/>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.4">
+        <v>122</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>20</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S33" t="s">
+        <v>34</v>
+      </c>
+      <c r="T33" t="s">
+        <v>46</v>
+      </c>
+      <c r="U33" t="s">
+        <v>47</v>
+      </c>
+      <c r="V33" t="s">
+        <v>48</v>
+      </c>
+      <c r="W33" t="s">
+        <v>49</v>
+      </c>
+      <c r="X33" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P34" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>59</v>
-      </c>
-      <c r="R34" t="s">
-        <v>60</v>
-      </c>
-      <c r="S34" t="s">
-        <v>61</v>
-      </c>
-      <c r="T34" t="s">
-        <v>62</v>
-      </c>
-      <c r="U34" t="s">
-        <v>63</v>
-      </c>
-      <c r="V34" t="s">
-        <v>64</v>
-      </c>
-      <c r="W34" t="s">
-        <v>22</v>
-      </c>
-      <c r="X34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.4">
+        <v>199</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H34" t="s">
+        <v>193</v>
+      </c>
+      <c r="I34" t="s">
+        <v>194</v>
+      </c>
+      <c r="J34" t="s">
+        <v>195</v>
+      </c>
+      <c r="K34" t="s">
+        <v>196</v>
+      </c>
+      <c r="L34" t="s">
+        <v>197</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R34" s="4"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2650,98 +2681,193 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H35" t="s">
+        <v>202</v>
+      </c>
+      <c r="I35" t="s">
+        <v>203</v>
+      </c>
+      <c r="J35" t="s">
+        <v>204</v>
+      </c>
+      <c r="R35" s="4"/>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="P35" t="s">
+      <c r="E36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q36" t="s">
         <v>20</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="R36" t="s">
+        <v>56</v>
+      </c>
+      <c r="S36" t="s">
+        <v>57</v>
+      </c>
+      <c r="T36" t="s">
+        <v>58</v>
+      </c>
+      <c r="U36" t="s">
         <v>59</v>
       </c>
-      <c r="R35" t="s">
+      <c r="V36" t="s">
         <v>60</v>
       </c>
-      <c r="S35" t="s">
+      <c r="W36" t="s">
         <v>61</v>
       </c>
-      <c r="T35" t="s">
+      <c r="X36" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="U35" t="s">
-        <v>63</v>
-      </c>
-      <c r="V35" t="s">
-        <v>64</v>
-      </c>
-      <c r="W35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>132</v>
-      </c>
-      <c r="B36" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G36" t="s">
-        <v>214</v>
-      </c>
-      <c r="H36" t="s">
-        <v>215</v>
-      </c>
-      <c r="I36" t="s">
-        <v>216</v>
-      </c>
-      <c r="J36" t="s">
-        <v>217</v>
-      </c>
-      <c r="K36" t="s">
-        <v>218</v>
-      </c>
-      <c r="L36" s="8"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" t="s">
-        <v>160</v>
-      </c>
-      <c r="C37" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" t="s">
-        <v>164</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>165</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G37" s="8"/>
+        <v>148</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>20</v>
+      </c>
+      <c r="R37" t="s">
+        <v>56</v>
+      </c>
+      <c r="S37" t="s">
+        <v>57</v>
+      </c>
+      <c r="T37" t="s">
+        <v>58</v>
+      </c>
+      <c r="U37" t="s">
+        <v>59</v>
+      </c>
+      <c r="V37" t="s">
+        <v>60</v>
+      </c>
+      <c r="W37" t="s">
+        <v>61</v>
+      </c>
+      <c r="X37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" t="s">
+        <v>151</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H38" t="s">
+        <v>202</v>
+      </c>
+      <c r="I38" t="s">
+        <v>203</v>
+      </c>
+      <c r="J38" t="s">
+        <v>204</v>
+      </c>
+      <c r="K38" t="s">
+        <v>205</v>
+      </c>
+      <c r="L38" t="s">
+        <v>206</v>
+      </c>
+      <c r="M38" s="8"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2762,203 +2888,203 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
         <v>73</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
         <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>81</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
         <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>81</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
         <v>78</v>
-      </c>
-      <c r="C15" t="s">
-        <v>81</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
@@ -2969,13 +3095,13 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
@@ -2986,13 +3112,13 @@
         <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
@@ -3003,13 +3129,13 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -3020,13 +3146,13 @@
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
@@ -3034,16 +3160,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
@@ -3054,13 +3180,13 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
@@ -3071,7 +3197,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -3088,13 +3214,13 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
@@ -3105,13 +3231,13 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
@@ -3122,13 +3248,13 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
         <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
@@ -3142,7 +3268,7 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
@@ -3156,7 +3282,7 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
@@ -3170,7 +3296,7 @@
         <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all finished test for API functions, add controller(logIn, logOut, isLogIn).
</commit_message>
<xml_diff>
--- a/documents/API 명세서.xlsx
+++ b/documents/API 명세서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\TJSManager_main\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF51F69B-DDB0-4F89-BCC8-1759A59690A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF1B44-8729-4685-85CC-B80736308A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="249">
   <si>
     <t>시스템</t>
   </si>
@@ -158,9 +158,6 @@
     <t>모든 입고 신청서 조회</t>
   </si>
   <si>
-    <t>req_num: int</t>
-  </si>
-  <si>
     <t>한 입고 신청서 조회</t>
   </si>
   <si>
@@ -170,12 +167,6 @@
     <t>입고 신청서 삭제</t>
   </si>
   <si>
-    <t>모든 최종 입고 신청 이력 조회</t>
-  </si>
-  <si>
-    <t>한 최종 입고 신청 이력 조회</t>
-  </si>
-  <si>
     <t>/item/stock</t>
   </si>
   <si>
@@ -411,26 +402,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/item/req_in_warehouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/item/req_in_warehouse/{report_num}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getAllReqInWarehouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/item/req_in_warehouse/{req_num}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getOneReqInWarehouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>/item/in_warehouse_report/{report_num}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -471,10 +442,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>모든 물품별 구매자 기록</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>getAllSalesConsumer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -511,10 +478,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>한 물품별 구매자 기록</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>getOneSalesConsumer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -672,10 +635,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>salesNum: Long(1)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>consumerGender: String("m"/"f")</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -736,10 +695,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>입고 신청 최종 승인 | 최종 입고 신청 이력 생성</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>inCnt: int(3 등)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -802,10 +757,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>물품별 구매자 기록 생성</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>판매 이력 기록 생성</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -879,6 +830,90 @@
   </si>
   <si>
     <t>storeTelNum: String(지점 전화번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매자 기록 생성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 구매자 기록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 구매자 기록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매자 기록 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateSalesConsumer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매 이력 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateSalesRecord</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HRM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employeeLogin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemNum: Long(물품 번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>empNum: String(직원 번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>empPassword: String(직원 비밀번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employee/log_out</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employee/log_in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employeeLogIOut</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employee/is_log_in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 여부 확인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employeeIsLogIn</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -968,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -980,6 +1015,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1294,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1309,15 +1350,15 @@
     <col min="5" max="5" width="29.19921875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.19921875" style="4" customWidth="1"/>
     <col min="7" max="7" width="47.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.8984375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.59765625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.69921875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.19921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.19921875" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="34.19921875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="41.8984375" bestFit="1" customWidth="1"/>
@@ -1345,10 +1386,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>5</v>
@@ -1364,152 +1405,93 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>106</v>
+    <row r="2" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="I2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" t="s">
-        <v>173</v>
-      </c>
-      <c r="K2" t="s">
-        <v>174</v>
-      </c>
-      <c r="L2" t="s">
-        <v>175</v>
-      </c>
-      <c r="N2"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="N3"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U3" t="s">
-        <v>14</v>
-      </c>
-      <c r="V3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W3" t="s">
-        <v>16</v>
-      </c>
-      <c r="X3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>23</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
+      <c r="A4" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="N4"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4" t="s">
-        <v>12</v>
-      </c>
-      <c r="T4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" t="s">
-        <v>14</v>
-      </c>
-      <c r="V4" t="s">
-        <v>15</v>
-      </c>
-      <c r="W4" t="s">
-        <v>16</v>
-      </c>
-      <c r="X4" t="s">
-        <v>22</v>
+        <v>247</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.4">
@@ -1520,62 +1502,88 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="J5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="K5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="L5" t="s">
-        <v>175</v>
-      </c>
-      <c r="N5"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>28</v>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="O6" s="6"/>
+        <v>208</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
@@ -1585,693 +1593,692 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>176</v>
+        <v>106</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H7" t="s">
-        <v>177</v>
-      </c>
-      <c r="I7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J7" t="s">
-        <v>179</v>
-      </c>
-      <c r="K7" t="s">
-        <v>180</v>
-      </c>
-      <c r="N7"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="4"/>
+        <v>208</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" t="s">
+        <v>21</v>
+      </c>
+      <c r="S7" t="s">
+        <v>12</v>
+      </c>
+      <c r="T7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" t="s">
+        <v>15</v>
+      </c>
+      <c r="W7" t="s">
+        <v>16</v>
+      </c>
+      <c r="X7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>26</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>184</v>
+        <v>27</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="N8"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" t="s">
-        <v>136</v>
+        <v>208</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K8" t="s">
+        <v>164</v>
+      </c>
+      <c r="L8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>187</v>
+        <v>29</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="N9"/>
+        <v>208</v>
+      </c>
       <c r="O9" s="6"/>
-      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" t="s">
         <v>167</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="N10"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="4"/>
+      <c r="I10" t="s">
+        <v>168</v>
+      </c>
+      <c r="J10" t="s">
+        <v>169</v>
+      </c>
+      <c r="K10" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>229</v>
+        <v>174</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N11"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="4"/>
+        <v>208</v>
+      </c>
+      <c r="H11"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>232</v>
+        <v>176</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>231</v>
+        <v>177</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>227</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="H12"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C13" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="K13" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N14" s="4"/>
+        <v>214</v>
+      </c>
+      <c r="H14"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>217</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="J15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L15" t="s">
-        <v>192</v>
-      </c>
-      <c r="N15"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="4"/>
+        <v>219</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H15"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="4"/>
+      <c r="P15"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H17"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J18" t="s">
+        <v>180</v>
+      </c>
+      <c r="K18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="P19" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>131</v>
+      </c>
+      <c r="R19" t="s">
         <v>132</v>
       </c>
-      <c r="B16" t="s">
+      <c r="S19" t="s">
         <v>133</v>
       </c>
-      <c r="C16" t="s">
+      <c r="T19" t="s">
+        <v>134</v>
+      </c>
+      <c r="U19" t="s">
         <v>135</v>
       </c>
-      <c r="D16" t="s">
+      <c r="V19" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="6" t="s">
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
         <v>137</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="D20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="N16"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="4" t="s">
+      <c r="G20" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="Q20" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="R20" t="s">
+        <v>132</v>
+      </c>
+      <c r="S20" t="s">
+        <v>133</v>
+      </c>
+      <c r="T20" t="s">
+        <v>134</v>
+      </c>
+      <c r="U20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I21" t="s">
+        <v>179</v>
+      </c>
+      <c r="J21" t="s">
+        <v>180</v>
+      </c>
+      <c r="K21" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q21" s="4"/>
+    </row>
+    <row r="22" spans="1:29" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="Q22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="F23" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="R16" t="s">
+      <c r="G23" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="R23" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="S23" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T23" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U23" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V23" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W23" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="X23" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="F24" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="N17"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="R17" t="s">
-        <v>141</v>
-      </c>
-      <c r="S17" t="s">
-        <v>142</v>
-      </c>
-      <c r="T17" t="s">
-        <v>143</v>
-      </c>
-      <c r="U17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="O18" s="7"/>
-      <c r="Q18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="R19" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="S19" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="T19" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="U19" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="V19" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="W19" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="X19" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20" s="6"/>
-      <c r="Q20" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="R20" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="S20" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="T20" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="U20" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="V20" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="W20" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="X20" s="8"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J21" t="s">
-        <v>200</v>
-      </c>
-      <c r="K21" t="s">
-        <v>201</v>
-      </c>
-      <c r="L21" t="s">
-        <v>202</v>
-      </c>
-      <c r="M21" t="s">
-        <v>203</v>
-      </c>
-      <c r="N21"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" s="4"/>
-      <c r="N22"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>20</v>
-      </c>
-      <c r="R22" t="s">
-        <v>116</v>
-      </c>
-      <c r="S22" t="s">
-        <v>34</v>
-      </c>
-      <c r="T22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U22" t="s">
-        <v>39</v>
-      </c>
-      <c r="V22" t="s">
-        <v>22</v>
-      </c>
-      <c r="W22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="N23"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" t="s">
-        <v>20</v>
-      </c>
-      <c r="R23" t="s">
-        <v>116</v>
-      </c>
-      <c r="S23" t="s">
-        <v>34</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U23" t="s">
-        <v>39</v>
-      </c>
-      <c r="V23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J24" t="s">
-        <v>200</v>
-      </c>
-      <c r="K24" t="s">
-        <v>201</v>
-      </c>
-      <c r="L24" t="s">
-        <v>202</v>
-      </c>
-      <c r="M24" t="s">
-        <v>203</v>
-      </c>
+      <c r="G24" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
       <c r="N24"/>
       <c r="O24" s="6"/>
-      <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
+      <c r="Q24" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="S24" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="T24" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="U24" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="V24" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="W24" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="X24" s="8"/>
+    </row>
+    <row r="25" spans="1:29" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.4">
+        <v>233</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25" s="6"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2279,19 +2286,37 @@
         <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J26" t="s">
+        <v>189</v>
+      </c>
+      <c r="K26" t="s">
+        <v>190</v>
+      </c>
+      <c r="L26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2299,43 +2324,46 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="O27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="P27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>20</v>
       </c>
-      <c r="Q27" t="s">
-        <v>41</v>
-      </c>
       <c r="R27" t="s">
+        <v>113</v>
+      </c>
+      <c r="S27" t="s">
         <v>34</v>
       </c>
-      <c r="S27" s="3" t="s">
+      <c r="T27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>39</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>22</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2343,37 +2371,40 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="P28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q28" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" t="s">
-        <v>41</v>
-      </c>
       <c r="R28" t="s">
+        <v>113</v>
+      </c>
+      <c r="S28" t="s">
         <v>34</v>
       </c>
-      <c r="S28" s="3" t="s">
+      <c r="T28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>39</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2381,37 +2412,40 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" t="s">
-        <v>205</v>
-      </c>
-      <c r="H29" t="s">
-        <v>206</v>
-      </c>
-      <c r="I29" t="s">
-        <v>207</v>
+        <v>42</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="J29" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="K29" t="s">
-        <v>209</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.4">
+        <v>190</v>
+      </c>
+      <c r="L29" t="s">
+        <v>191</v>
+      </c>
+      <c r="M29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2419,55 +2453,26 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="O30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P30" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R30" t="s">
-        <v>34</v>
-      </c>
-      <c r="S30" t="s">
-        <v>49</v>
-      </c>
-      <c r="T30" t="s">
-        <v>50</v>
-      </c>
-      <c r="U30" t="s">
-        <v>51</v>
-      </c>
-      <c r="V30" t="s">
-        <v>52</v>
-      </c>
-      <c r="W30" t="s">
-        <v>53</v>
-      </c>
-      <c r="X30" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="4"/>
+      <c r="P30"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2475,88 +2480,105 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>210</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="J31" t="s">
+        <v>193</v>
+      </c>
+      <c r="K31" t="s">
+        <v>194</v>
+      </c>
+      <c r="L31" t="s">
+        <v>195</v>
+      </c>
+      <c r="M31" t="s">
+        <v>196</v>
+      </c>
+      <c r="N31" t="s">
+        <v>197</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="P31" t="s">
+      <c r="E32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q32" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="3" t="s">
+      <c r="R32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S32" t="s">
         <v>34</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T32" t="s">
+        <v>46</v>
+      </c>
+      <c r="U32" t="s">
+        <v>47</v>
+      </c>
+      <c r="V32" t="s">
+        <v>48</v>
+      </c>
+      <c r="W32" t="s">
         <v>49</v>
       </c>
-      <c r="T31" t="s">
+      <c r="X32" t="s">
         <v>50</v>
       </c>
-      <c r="U31" t="s">
+      <c r="Y32" t="s">
         <v>51</v>
       </c>
-      <c r="V31" t="s">
-        <v>52</v>
-      </c>
-      <c r="W31" t="s">
-        <v>53</v>
-      </c>
-      <c r="X31" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA31" t="s">
+      <c r="AB32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>132</v>
-      </c>
-      <c r="B32" t="s">
-        <v>160</v>
-      </c>
-      <c r="C32" t="s">
-        <v>210</v>
-      </c>
-      <c r="D32" t="s">
-        <v>161</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="G32" t="s">
-        <v>205</v>
-      </c>
-      <c r="H32" t="s">
-        <v>206</v>
-      </c>
-      <c r="I32" t="s">
-        <v>207</v>
-      </c>
-      <c r="J32" t="s">
-        <v>208</v>
-      </c>
-      <c r="K32" t="s">
-        <v>209</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q32" s="4"/>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="AC32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2564,85 +2586,94 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>17</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>213</v>
+        <v>53</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G33" t="s">
-        <v>214</v>
-      </c>
-      <c r="H33" t="s">
-        <v>215</v>
-      </c>
-      <c r="I33" t="s">
-        <v>216</v>
-      </c>
-      <c r="J33" t="s">
-        <v>217</v>
-      </c>
-      <c r="K33" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q33" s="4"/>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.4">
+        <v>122</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>20</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S33" t="s">
+        <v>34</v>
+      </c>
+      <c r="T33" t="s">
+        <v>46</v>
+      </c>
+      <c r="U33" t="s">
+        <v>47</v>
+      </c>
+      <c r="V33" t="s">
+        <v>48</v>
+      </c>
+      <c r="W33" t="s">
+        <v>49</v>
+      </c>
+      <c r="X33" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P34" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>59</v>
-      </c>
-      <c r="R34" t="s">
-        <v>60</v>
-      </c>
-      <c r="S34" t="s">
-        <v>61</v>
-      </c>
-      <c r="T34" t="s">
-        <v>62</v>
-      </c>
-      <c r="U34" t="s">
-        <v>63</v>
-      </c>
-      <c r="V34" t="s">
-        <v>64</v>
-      </c>
-      <c r="W34" t="s">
-        <v>22</v>
-      </c>
-      <c r="X34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.4">
+        <v>199</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H34" t="s">
+        <v>193</v>
+      </c>
+      <c r="I34" t="s">
+        <v>194</v>
+      </c>
+      <c r="J34" t="s">
+        <v>195</v>
+      </c>
+      <c r="K34" t="s">
+        <v>196</v>
+      </c>
+      <c r="L34" t="s">
+        <v>197</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R34" s="4"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2650,98 +2681,193 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H35" t="s">
+        <v>202</v>
+      </c>
+      <c r="I35" t="s">
+        <v>203</v>
+      </c>
+      <c r="J35" t="s">
+        <v>204</v>
+      </c>
+      <c r="R35" s="4"/>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="P35" t="s">
+      <c r="E36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q36" t="s">
         <v>20</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="R36" t="s">
+        <v>56</v>
+      </c>
+      <c r="S36" t="s">
+        <v>57</v>
+      </c>
+      <c r="T36" t="s">
+        <v>58</v>
+      </c>
+      <c r="U36" t="s">
         <v>59</v>
       </c>
-      <c r="R35" t="s">
+      <c r="V36" t="s">
         <v>60</v>
       </c>
-      <c r="S35" t="s">
+      <c r="W36" t="s">
         <v>61</v>
       </c>
-      <c r="T35" t="s">
+      <c r="X36" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="U35" t="s">
-        <v>63</v>
-      </c>
-      <c r="V35" t="s">
-        <v>64</v>
-      </c>
-      <c r="W35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>132</v>
-      </c>
-      <c r="B36" t="s">
-        <v>160</v>
-      </c>
-      <c r="C36" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G36" t="s">
-        <v>214</v>
-      </c>
-      <c r="H36" t="s">
-        <v>215</v>
-      </c>
-      <c r="I36" t="s">
-        <v>216</v>
-      </c>
-      <c r="J36" t="s">
-        <v>217</v>
-      </c>
-      <c r="K36" t="s">
-        <v>218</v>
-      </c>
-      <c r="L36" s="8"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" t="s">
-        <v>160</v>
-      </c>
-      <c r="C37" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" t="s">
-        <v>164</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>165</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G37" s="8"/>
+        <v>148</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>20</v>
+      </c>
+      <c r="R37" t="s">
+        <v>56</v>
+      </c>
+      <c r="S37" t="s">
+        <v>57</v>
+      </c>
+      <c r="T37" t="s">
+        <v>58</v>
+      </c>
+      <c r="U37" t="s">
+        <v>59</v>
+      </c>
+      <c r="V37" t="s">
+        <v>60</v>
+      </c>
+      <c r="W37" t="s">
+        <v>61</v>
+      </c>
+      <c r="X37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" t="s">
+        <v>151</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H38" t="s">
+        <v>202</v>
+      </c>
+      <c r="I38" t="s">
+        <v>203</v>
+      </c>
+      <c r="J38" t="s">
+        <v>204</v>
+      </c>
+      <c r="K38" t="s">
+        <v>205</v>
+      </c>
+      <c r="L38" t="s">
+        <v>206</v>
+      </c>
+      <c r="M38" s="8"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2762,203 +2888,203 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
         <v>73</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
         <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>81</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
         <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>81</v>
       </c>
       <c r="D14" t="s">
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
         <v>78</v>
-      </c>
-      <c r="C15" t="s">
-        <v>81</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
@@ -2969,13 +3095,13 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
@@ -2986,13 +3112,13 @@
         <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
@@ -3003,13 +3129,13 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -3020,13 +3146,13 @@
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
@@ -3034,16 +3160,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
@@ -3054,13 +3180,13 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
@@ -3071,7 +3197,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -3088,13 +3214,13 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
@@ -3105,13 +3231,13 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
@@ -3122,13 +3248,13 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
         <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
@@ -3142,7 +3268,7 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
@@ -3156,7 +3282,7 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
@@ -3170,7 +3296,7 @@
         <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify documents/api명세서, add API Employee CRUD.
</commit_message>
<xml_diff>
--- a/documents/API 명세서.xlsx
+++ b/documents/API 명세서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\TJSManager_main\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF1B44-8729-4685-85CC-B80736308A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED38A41-84DE-4B6A-820E-CECF0111E6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="279">
   <si>
     <t>시스템</t>
   </si>
@@ -881,22 +881,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>empNum: String(직원 번호)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>empPassword: String(직원 비밀번호)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>employee/log_out</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>employee/log_in</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>로그아웃</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -905,15 +893,146 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>employee/is_log_in</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인 여부 확인</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>employeeIsLogIn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>통계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/consumer_gender/all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 성별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupByGender</t>
+  </si>
+  <si>
+    <t>/statistics/consumer_age/all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 나이대별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupByAge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/consumer_hour/all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 시간대별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupByHour</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>empNum: Long(직원 번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/log_in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/log_out</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/is_log_in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 정보 생성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>createEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 직원 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/{emp_num}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 직원 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getOneEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 정보 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 정보 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>deleteEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name: String(이름)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>job: String("점장", "일반" 등)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gender: String("m", "f")</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>birthDate: String(생년월일)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>phoneNum: String(전화번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hireDate: String(입사일)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>salary: int(월급)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wage: int(시급)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1335,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC39"/>
+  <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1359,17 +1478,18 @@
     <col min="14" max="14" width="21.19921875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.5" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.19921875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="41.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="44.09765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.19921875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.19921875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.19921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="41.8984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="44.09765625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1401,11 +1521,13 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
       <c r="O1" s="10"/>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
         <v>235</v>
       </c>
@@ -1413,7 +1535,7 @@
         <v>236</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>157</v>
@@ -1428,10 +1550,10 @@
         <v>208</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>241</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
@@ -1439,8 +1561,10 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="15"/>
-    </row>
-    <row r="3" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>235</v>
       </c>
@@ -1448,16 +1572,16 @@
         <v>236</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>157</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>208</v>
@@ -1470,8 +1594,10 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="15"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
         <v>235</v>
       </c>
@@ -1479,222 +1605,202 @@
         <v>236</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A5" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I5" t="s">
-        <v>162</v>
-      </c>
-      <c r="J5" t="s">
-        <v>163</v>
-      </c>
-      <c r="K5" t="s">
-        <v>164</v>
-      </c>
-      <c r="L5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
+        <v>260</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A6" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" t="s">
-        <v>12</v>
-      </c>
-      <c r="T6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V6" t="s">
-        <v>15</v>
-      </c>
-      <c r="W6" t="s">
-        <v>16</v>
-      </c>
-      <c r="X6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
+        <v>262</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A7" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>20</v>
-      </c>
-      <c r="R7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S7" t="s">
-        <v>12</v>
-      </c>
-      <c r="T7" t="s">
-        <v>13</v>
-      </c>
-      <c r="U7" t="s">
-        <v>14</v>
-      </c>
-      <c r="V7" t="s">
-        <v>15</v>
-      </c>
-      <c r="W7" t="s">
-        <v>16</v>
-      </c>
-      <c r="X7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
+        <v>265</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I8" t="s">
-        <v>162</v>
-      </c>
-      <c r="J8" t="s">
-        <v>163</v>
-      </c>
-      <c r="K8" t="s">
-        <v>164</v>
-      </c>
-      <c r="L8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>267</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A9" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+        <v>268</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1702,777 +1808,791 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I10" t="s">
+        <v>162</v>
+      </c>
+      <c r="J10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" t="s">
+        <v>164</v>
+      </c>
+      <c r="L10" t="s">
+        <v>165</v>
+      </c>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S11" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" t="s">
+        <v>12</v>
+      </c>
+      <c r="V11" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" t="s">
+        <v>14</v>
+      </c>
+      <c r="X11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="R12" s="4"/>
+      <c r="S12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T12" t="s">
+        <v>21</v>
+      </c>
+      <c r="U12" t="s">
+        <v>12</v>
+      </c>
+      <c r="V12" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" t="s">
+        <v>14</v>
+      </c>
+      <c r="X12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I13" t="s">
+        <v>162</v>
+      </c>
+      <c r="J13" t="s">
+        <v>163</v>
+      </c>
+      <c r="K13" t="s">
+        <v>164</v>
+      </c>
+      <c r="L13" t="s">
+        <v>165</v>
+      </c>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G15" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H15" t="s">
         <v>167</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I15" t="s">
         <v>168</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J15" t="s">
         <v>169</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K15" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>171</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>172</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>159</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D16" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="G16" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16"/>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>171</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B17" t="s">
         <v>172</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C17" t="s">
         <v>175</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D17" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" t="s">
-        <v>210</v>
-      </c>
-      <c r="C15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D15" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H15"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="4"/>
-      <c r="P15"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C16" t="s">
-        <v>217</v>
-      </c>
-      <c r="D16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B17" t="s">
-        <v>210</v>
-      </c>
-      <c r="C17" t="s">
-        <v>217</v>
-      </c>
-      <c r="D17" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>223</v>
-      </c>
       <c r="G17" s="8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="H17"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17"/>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>211</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>109</v>
+        <v>212</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="I18" t="s">
-        <v>179</v>
-      </c>
-      <c r="J18" t="s">
-        <v>180</v>
-      </c>
-      <c r="K18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.4">
+        <v>208</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="D19" t="s">
         <v>128</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>129</v>
+        <v>216</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="P19" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>131</v>
-      </c>
-      <c r="R19" t="s">
-        <v>132</v>
-      </c>
-      <c r="S19" t="s">
-        <v>133</v>
-      </c>
-      <c r="T19" t="s">
-        <v>134</v>
-      </c>
-      <c r="U19" t="s">
-        <v>135</v>
-      </c>
-      <c r="V19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="H19"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="D20" t="s">
         <v>128</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="Q20" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="R20" t="s">
-        <v>132</v>
-      </c>
-      <c r="S20" t="s">
-        <v>133</v>
-      </c>
-      <c r="T20" t="s">
-        <v>134</v>
-      </c>
-      <c r="U20" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="H20"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
         <v>151</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" t="s">
+        <v>210</v>
+      </c>
+      <c r="C22" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" t="s">
+        <v>179</v>
+      </c>
+      <c r="J23" t="s">
+        <v>180</v>
+      </c>
+      <c r="K23" t="s">
+        <v>181</v>
+      </c>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="R24" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="S24" t="s">
+        <v>131</v>
+      </c>
+      <c r="T24" t="s">
+        <v>132</v>
+      </c>
+      <c r="U24" t="s">
+        <v>133</v>
+      </c>
+      <c r="V24" t="s">
+        <v>134</v>
+      </c>
+      <c r="W24" t="s">
+        <v>135</v>
+      </c>
+      <c r="X24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T25" t="s">
+        <v>132</v>
+      </c>
+      <c r="U25" t="s">
+        <v>133</v>
+      </c>
+      <c r="V25" t="s">
+        <v>134</v>
+      </c>
+      <c r="W25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H21" s="4" t="s">
+      <c r="G26" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I26" t="s">
         <v>179</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J26" t="s">
         <v>180</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K26" t="s">
         <v>181</v>
       </c>
-      <c r="Q21" s="4"/>
-    </row>
-    <row r="22" spans="1:29" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" spans="1:26" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="H22" s="2" t="s">
+      <c r="G27" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="O22" s="7"/>
-      <c r="Q22" s="2" t="s">
+      <c r="O27" s="7"/>
+      <c r="S27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R22" s="2" t="s">
+      <c r="T27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="U27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="8" t="s">
+    <row r="28" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B28" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="O23" s="6"/>
-      <c r="P23" s="4" t="s">
+      <c r="G28" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="O28" s="6"/>
+      <c r="R28" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="Q23" s="8" t="s">
+      <c r="S28" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="R23" s="8" t="s">
+      <c r="T28" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="S23" s="8" t="s">
+      <c r="U28" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T23" s="8" t="s">
+      <c r="V28" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="U23" s="8" t="s">
+      <c r="W28" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="V23" s="8" t="s">
+      <c r="X28" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="W23" s="8" t="s">
+      <c r="Y28" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X23" s="8" t="s">
+      <c r="Z28" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="8" t="s">
+    <row r="29" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G24" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24" s="6"/>
-      <c r="Q24" s="8" t="s">
+      <c r="G29" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29" s="6"/>
+      <c r="S29" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="R24" s="8" t="s">
+      <c r="T29" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="S24" s="8" t="s">
+      <c r="U29" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T24" s="8" t="s">
+      <c r="V29" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="U24" s="8" t="s">
+      <c r="W29" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="V24" s="8" t="s">
+      <c r="X29" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="W24" s="8" t="s">
+      <c r="Y29" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X24" s="8"/>
-    </row>
-    <row r="25" spans="1:29" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="8" t="s">
+      <c r="Z29" s="8"/>
+    </row>
+    <row r="30" spans="1:26" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B30" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H25" s="2" t="s">
+      <c r="G30" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25" s="6"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="J26" t="s">
-        <v>189</v>
-      </c>
-      <c r="K26" t="s">
-        <v>190</v>
-      </c>
-      <c r="L26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="P27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>20</v>
-      </c>
-      <c r="R27" t="s">
-        <v>113</v>
-      </c>
-      <c r="S27" t="s">
-        <v>34</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U27" t="s">
-        <v>39</v>
-      </c>
-      <c r="V27" t="s">
-        <v>22</v>
-      </c>
-      <c r="W27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>20</v>
-      </c>
-      <c r="R28" t="s">
-        <v>113</v>
-      </c>
-      <c r="S28" t="s">
-        <v>34</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U28" t="s">
-        <v>39</v>
-      </c>
-      <c r="V28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="J29" t="s">
-        <v>189</v>
-      </c>
-      <c r="K29" t="s">
-        <v>190</v>
-      </c>
-      <c r="L29" t="s">
-        <v>191</v>
-      </c>
-      <c r="M29" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H30"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="4"/>
-      <c r="P30"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30" s="6"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="8"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2480,46 +2600,38 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>120</v>
+        <v>37</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H31" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="I31" s="8" t="s">
+      <c r="H31" s="4" t="s">
         <v>187</v>
       </c>
+      <c r="I31" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="J31" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K31" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="L31" t="s">
-        <v>195</v>
-      </c>
-      <c r="M31" t="s">
-        <v>196</v>
-      </c>
-      <c r="N31" t="s">
-        <v>197</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.4">
+        <v>191</v>
+      </c>
+      <c r="R31" s="4"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2527,58 +2639,46 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>208</v>
       </c>
       <c r="P32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>20</v>
       </c>
-      <c r="R32" s="3" t="s">
+      <c r="S32" t="s">
+        <v>113</v>
+      </c>
+      <c r="T32" t="s">
+        <v>34</v>
+      </c>
+      <c r="U32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S32" t="s">
-        <v>34</v>
-      </c>
-      <c r="T32" t="s">
-        <v>46</v>
-      </c>
-      <c r="U32" t="s">
-        <v>47</v>
-      </c>
       <c r="V32" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="W32" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="X32" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2586,94 +2686,81 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>122</v>
+        <v>41</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>20</v>
       </c>
-      <c r="R33" s="3" t="s">
+      <c r="S33" t="s">
+        <v>113</v>
+      </c>
+      <c r="T33" t="s">
+        <v>34</v>
+      </c>
+      <c r="U33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S33" t="s">
-        <v>34</v>
-      </c>
-      <c r="T33" t="s">
-        <v>46</v>
-      </c>
-      <c r="U33" t="s">
-        <v>47</v>
-      </c>
       <c r="V33" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="W33" t="s">
-        <v>49</v>
-      </c>
-      <c r="X33" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>200</v>
+        <v>42</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H34" t="s">
-        <v>193</v>
-      </c>
-      <c r="I34" t="s">
-        <v>194</v>
+      <c r="H34" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="J34" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="K34" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="L34" t="s">
-        <v>197</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="R34" s="4"/>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.4">
+        <v>191</v>
+      </c>
+      <c r="M34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2681,32 +2768,27 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>157</v>
+        <v>28</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>158</v>
+        <v>43</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H35" t="s">
-        <v>202</v>
-      </c>
-      <c r="I35" t="s">
-        <v>203</v>
-      </c>
-      <c r="J35" t="s">
-        <v>204</v>
-      </c>
-      <c r="R35" s="4"/>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="H35"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="4"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2714,52 +2796,46 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>147</v>
+        <v>45</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="P36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>20</v>
-      </c>
-      <c r="R36" t="s">
-        <v>56</v>
-      </c>
-      <c r="S36" t="s">
-        <v>57</v>
-      </c>
-      <c r="T36" t="s">
-        <v>58</v>
-      </c>
-      <c r="U36" t="s">
-        <v>59</v>
-      </c>
-      <c r="V36" t="s">
-        <v>60</v>
-      </c>
-      <c r="W36" t="s">
-        <v>61</v>
-      </c>
-      <c r="X36" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="H36" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="J36" t="s">
+        <v>193</v>
+      </c>
+      <c r="K36" t="s">
+        <v>194</v>
+      </c>
+      <c r="L36" t="s">
+        <v>195</v>
+      </c>
+      <c r="M36" t="s">
+        <v>196</v>
+      </c>
+      <c r="N36" t="s">
+        <v>197</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -2767,85 +2843,111 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>148</v>
+        <v>52</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="P37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R37" t="s">
         <v>20</v>
       </c>
-      <c r="R37" t="s">
-        <v>56</v>
-      </c>
-      <c r="S37" t="s">
-        <v>57</v>
+      <c r="S37" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="T37" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="U37" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="V37" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="W37" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="X37" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.4">
+        <v>49</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="D38" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>153</v>
+        <v>53</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H38" t="s">
-        <v>202</v>
-      </c>
-      <c r="I38" t="s">
-        <v>203</v>
-      </c>
-      <c r="J38" t="s">
-        <v>204</v>
-      </c>
-      <c r="K38" t="s">
-        <v>205</v>
-      </c>
-      <c r="L38" t="s">
-        <v>206</v>
-      </c>
-      <c r="M38" s="8"/>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="R38" t="s">
+        <v>20</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T38" t="s">
+        <v>34</v>
+      </c>
+      <c r="U38" t="s">
+        <v>46</v>
+      </c>
+      <c r="V38" t="s">
+        <v>47</v>
+      </c>
+      <c r="W38" t="s">
+        <v>48</v>
+      </c>
+      <c r="X38" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>124</v>
       </c>
@@ -2853,21 +2955,302 @@
         <v>150</v>
       </c>
       <c r="C39" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" t="s">
+        <v>193</v>
+      </c>
+      <c r="I39" t="s">
+        <v>194</v>
+      </c>
+      <c r="J39" t="s">
+        <v>195</v>
+      </c>
+      <c r="K39" t="s">
+        <v>196</v>
+      </c>
+      <c r="L39" t="s">
+        <v>197</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="S39" s="4"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H40" t="s">
+        <v>202</v>
+      </c>
+      <c r="I40" t="s">
+        <v>203</v>
+      </c>
+      <c r="J40" t="s">
+        <v>204</v>
+      </c>
+      <c r="S40" s="4"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R41" t="s">
+        <v>20</v>
+      </c>
+      <c r="S41" t="s">
+        <v>56</v>
+      </c>
+      <c r="T41" t="s">
+        <v>57</v>
+      </c>
+      <c r="U41" t="s">
+        <v>58</v>
+      </c>
+      <c r="V41" t="s">
+        <v>59</v>
+      </c>
+      <c r="W41" t="s">
+        <v>60</v>
+      </c>
+      <c r="X41" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" t="s">
         <v>123</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="R42" t="s">
+        <v>20</v>
+      </c>
+      <c r="S42" t="s">
+        <v>56</v>
+      </c>
+      <c r="T42" t="s">
+        <v>57</v>
+      </c>
+      <c r="U42" t="s">
+        <v>58</v>
+      </c>
+      <c r="V42" t="s">
+        <v>59</v>
+      </c>
+      <c r="W42" t="s">
+        <v>60</v>
+      </c>
+      <c r="X42" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H43" t="s">
+        <v>202</v>
+      </c>
+      <c r="I43" t="s">
+        <v>203</v>
+      </c>
+      <c r="J43" t="s">
+        <v>204</v>
+      </c>
+      <c r="K43" t="s">
+        <v>205</v>
+      </c>
+      <c r="L43" t="s">
+        <v>206</v>
+      </c>
+      <c r="M43" s="8"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
         <v>154</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G39" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H39" s="8"/>
+      <c r="G44" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" t="s">
+        <v>245</v>
+      </c>
+      <c r="C45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" t="s">
+        <v>245</v>
+      </c>
+      <c r="C46" t="s">
+        <v>249</v>
+      </c>
+      <c r="D46" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" t="s">
+        <v>245</v>
+      </c>
+      <c r="C47" t="s">
+        <v>252</v>
+      </c>
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="G47" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
create Employee CRUD, modify employee/login null error.
</commit_message>
<xml_diff>
--- a/documents/API 명세서.xlsx
+++ b/documents/API 명세서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\TJSManager_main\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF1B44-8729-4685-85CC-B80736308A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED38A41-84DE-4B6A-820E-CECF0111E6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="279">
   <si>
     <t>시스템</t>
   </si>
@@ -881,22 +881,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>empNum: String(직원 번호)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>empPassword: String(직원 비밀번호)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>employee/log_out</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>employee/log_in</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>로그아웃</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -905,15 +893,146 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>employee/is_log_in</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인 여부 확인</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>employeeIsLogIn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>통계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/consumer_gender/all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 성별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupByGender</t>
+  </si>
+  <si>
+    <t>/statistics/consumer_age/all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 나이대별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupByAge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/consumer_hour/all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 시간대별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupByHour</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>empNum: Long(직원 번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/log_in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/log_out</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/is_log_in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 정보 생성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>createEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 직원 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/employee/{emp_num}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 직원 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getOneEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 정보 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 정보 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>deleteEmployee</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name: String(이름)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>job: String("점장", "일반" 등)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gender: String("m", "f")</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>birthDate: String(생년월일)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>phoneNum: String(전화번호)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hireDate: String(입사일)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>salary: int(월급)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wage: int(시급)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1335,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC39"/>
+  <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1359,17 +1478,18 @@
     <col min="14" max="14" width="21.19921875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.5" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.19921875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="41.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="44.09765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.19921875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.19921875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.19921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="41.8984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="44.09765625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1401,11 +1521,13 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
       <c r="O1" s="10"/>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
         <v>235</v>
       </c>
@@ -1413,7 +1535,7 @@
         <v>236</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>157</v>
@@ -1428,10 +1550,10 @@
         <v>208</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>241</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
@@ -1439,8 +1561,10 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="15"/>
-    </row>
-    <row r="3" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>235</v>
       </c>
@@ -1448,16 +1572,16 @@
         <v>236</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>157</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>208</v>
@@ -1470,8 +1594,10 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="15"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
         <v>235</v>
       </c>
@@ -1479,222 +1605,202 @@
         <v>236</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A5" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I5" t="s">
-        <v>162</v>
-      </c>
-      <c r="J5" t="s">
-        <v>163</v>
-      </c>
-      <c r="K5" t="s">
-        <v>164</v>
-      </c>
-      <c r="L5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
+        <v>260</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A6" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" t="s">
-        <v>12</v>
-      </c>
-      <c r="T6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V6" t="s">
-        <v>15</v>
-      </c>
-      <c r="W6" t="s">
-        <v>16</v>
-      </c>
-      <c r="X6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
+        <v>262</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A7" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>20</v>
-      </c>
-      <c r="R7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S7" t="s">
-        <v>12</v>
-      </c>
-      <c r="T7" t="s">
-        <v>13</v>
-      </c>
-      <c r="U7" t="s">
-        <v>14</v>
-      </c>
-      <c r="V7" t="s">
-        <v>15</v>
-      </c>
-      <c r="W7" t="s">
-        <v>16</v>
-      </c>
-      <c r="X7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
+        <v>265</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I8" t="s">
-        <v>162</v>
-      </c>
-      <c r="J8" t="s">
-        <v>163</v>
-      </c>
-      <c r="K8" t="s">
-        <v>164</v>
-      </c>
-      <c r="L8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>267</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A9" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+        <v>268</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1702,777 +1808,791 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I10" t="s">
+        <v>162</v>
+      </c>
+      <c r="J10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" t="s">
+        <v>164</v>
+      </c>
+      <c r="L10" t="s">
+        <v>165</v>
+      </c>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S11" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" t="s">
+        <v>12</v>
+      </c>
+      <c r="V11" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" t="s">
+        <v>14</v>
+      </c>
+      <c r="X11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="R12" s="4"/>
+      <c r="S12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T12" t="s">
+        <v>21</v>
+      </c>
+      <c r="U12" t="s">
+        <v>12</v>
+      </c>
+      <c r="V12" t="s">
+        <v>13</v>
+      </c>
+      <c r="W12" t="s">
+        <v>14</v>
+      </c>
+      <c r="X12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I13" t="s">
+        <v>162</v>
+      </c>
+      <c r="J13" t="s">
+        <v>163</v>
+      </c>
+      <c r="K13" t="s">
+        <v>164</v>
+      </c>
+      <c r="L13" t="s">
+        <v>165</v>
+      </c>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G15" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H15" t="s">
         <v>167</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I15" t="s">
         <v>168</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J15" t="s">
         <v>169</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K15" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>171</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>172</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>159</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D16" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="G16" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16"/>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>171</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B17" t="s">
         <v>172</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C17" t="s">
         <v>175</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D17" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" t="s">
-        <v>210</v>
-      </c>
-      <c r="C15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D15" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H15"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="4"/>
-      <c r="P15"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C16" t="s">
-        <v>217</v>
-      </c>
-      <c r="D16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B17" t="s">
-        <v>210</v>
-      </c>
-      <c r="C17" t="s">
-        <v>217</v>
-      </c>
-      <c r="D17" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>223</v>
-      </c>
       <c r="G17" s="8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="H17"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17"/>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>211</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>109</v>
+        <v>212</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="I18" t="s">
-        <v>179</v>
-      </c>
-      <c r="J18" t="s">
-        <v>180</v>
-      </c>
-      <c r="K18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.4">
+        <v>208</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="D19" t="s">
         <v>128</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>129</v>
+        <v>216</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="P19" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>131</v>
-      </c>
-      <c r="R19" t="s">
-        <v>132</v>
-      </c>
-      <c r="S19" t="s">
-        <v>133</v>
-      </c>
-      <c r="T19" t="s">
-        <v>134</v>
-      </c>
-      <c r="U19" t="s">
-        <v>135</v>
-      </c>
-      <c r="V19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="H19"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="D20" t="s">
         <v>128</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="Q20" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="R20" t="s">
-        <v>132</v>
-      </c>
-      <c r="S20" t="s">
-        <v>133</v>
-      </c>
-      <c r="T20" t="s">
-        <v>134</v>
-      </c>
-      <c r="U20" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="H20"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
         <v>151</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" t="s">
+        <v>210</v>
+      </c>
+      <c r="C22" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" t="s">
+        <v>179</v>
+      </c>
+      <c r="J23" t="s">
+        <v>180</v>
+      </c>
+      <c r="K23" t="s">
+        <v>181</v>
+      </c>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="R24" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="S24" t="s">
+        <v>131</v>
+      </c>
+      <c r="T24" t="s">
+        <v>132</v>
+      </c>
+      <c r="U24" t="s">
+        <v>133</v>
+      </c>
+      <c r="V24" t="s">
+        <v>134</v>
+      </c>
+      <c r="W24" t="s">
+        <v>135</v>
+      </c>
+      <c r="X24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T25" t="s">
+        <v>132</v>
+      </c>
+      <c r="U25" t="s">
+        <v>133</v>
+      </c>
+      <c r="V25" t="s">
+        <v>134</v>
+      </c>
+      <c r="W25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H21" s="4" t="s">
+      <c r="G26" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I26" t="s">
         <v>179</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J26" t="s">
         <v>180</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K26" t="s">
         <v>181</v>
       </c>
-      <c r="Q21" s="4"/>
-    </row>
-    <row r="22" spans="1:29" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" spans="1:26" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="H22" s="2" t="s">
+      <c r="G27" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="O22" s="7"/>
-      <c r="Q22" s="2" t="s">
+      <c r="O27" s="7"/>
+      <c r="S27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R22" s="2" t="s">
+      <c r="T27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="U27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="8" t="s">
+    <row r="28" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B28" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="O23" s="6"/>
-      <c r="P23" s="4" t="s">
+      <c r="G28" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="O28" s="6"/>
+      <c r="R28" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="Q23" s="8" t="s">
+      <c r="S28" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="R23" s="8" t="s">
+      <c r="T28" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="S23" s="8" t="s">
+      <c r="U28" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T23" s="8" t="s">
+      <c r="V28" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="U23" s="8" t="s">
+      <c r="W28" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="V23" s="8" t="s">
+      <c r="X28" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="W23" s="8" t="s">
+      <c r="Y28" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X23" s="8" t="s">
+      <c r="Z28" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="8" t="s">
+    <row r="29" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G24" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24" s="6"/>
-      <c r="Q24" s="8" t="s">
+      <c r="G29" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29" s="6"/>
+      <c r="S29" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="R24" s="8" t="s">
+      <c r="T29" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="S24" s="8" t="s">
+      <c r="U29" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T24" s="8" t="s">
+      <c r="V29" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="U24" s="8" t="s">
+      <c r="W29" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="V24" s="8" t="s">
+      <c r="X29" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="W24" s="8" t="s">
+      <c r="Y29" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X24" s="8"/>
-    </row>
-    <row r="25" spans="1:29" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="8" t="s">
+      <c r="Z29" s="8"/>
+    </row>
+    <row r="30" spans="1:26" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B30" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H25" s="2" t="s">
+      <c r="G30" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25" s="6"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="J26" t="s">
-        <v>189</v>
-      </c>
-      <c r="K26" t="s">
-        <v>190</v>
-      </c>
-      <c r="L26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="P27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>20</v>
-      </c>
-      <c r="R27" t="s">
-        <v>113</v>
-      </c>
-      <c r="S27" t="s">
-        <v>34</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U27" t="s">
-        <v>39</v>
-      </c>
-      <c r="V27" t="s">
-        <v>22</v>
-      </c>
-      <c r="W27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>20</v>
-      </c>
-      <c r="R28" t="s">
-        <v>113</v>
-      </c>
-      <c r="S28" t="s">
-        <v>34</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U28" t="s">
-        <v>39</v>
-      </c>
-      <c r="V28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="J29" t="s">
-        <v>189</v>
-      </c>
-      <c r="K29" t="s">
-        <v>190</v>
-      </c>
-      <c r="L29" t="s">
-        <v>191</v>
-      </c>
-      <c r="M29" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H30"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="4"/>
-      <c r="P30"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30" s="6"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="8"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2480,46 +2600,38 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>120</v>
+        <v>37</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H31" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="I31" s="8" t="s">
+      <c r="H31" s="4" t="s">
         <v>187</v>
       </c>
+      <c r="I31" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="J31" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K31" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="L31" t="s">
-        <v>195</v>
-      </c>
-      <c r="M31" t="s">
-        <v>196</v>
-      </c>
-      <c r="N31" t="s">
-        <v>197</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.4">
+        <v>191</v>
+      </c>
+      <c r="R31" s="4"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2527,58 +2639,46 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>208</v>
       </c>
       <c r="P32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>20</v>
       </c>
-      <c r="R32" s="3" t="s">
+      <c r="S32" t="s">
+        <v>113</v>
+      </c>
+      <c r="T32" t="s">
+        <v>34</v>
+      </c>
+      <c r="U32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S32" t="s">
-        <v>34</v>
-      </c>
-      <c r="T32" t="s">
-        <v>46</v>
-      </c>
-      <c r="U32" t="s">
-        <v>47</v>
-      </c>
       <c r="V32" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="W32" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="X32" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2586,94 +2686,81 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>122</v>
+        <v>41</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>20</v>
       </c>
-      <c r="R33" s="3" t="s">
+      <c r="S33" t="s">
+        <v>113</v>
+      </c>
+      <c r="T33" t="s">
+        <v>34</v>
+      </c>
+      <c r="U33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S33" t="s">
-        <v>34</v>
-      </c>
-      <c r="T33" t="s">
-        <v>46</v>
-      </c>
-      <c r="U33" t="s">
-        <v>47</v>
-      </c>
       <c r="V33" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="W33" t="s">
-        <v>49</v>
-      </c>
-      <c r="X33" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>200</v>
+        <v>42</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H34" t="s">
-        <v>193</v>
-      </c>
-      <c r="I34" t="s">
-        <v>194</v>
+      <c r="H34" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="J34" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="K34" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="L34" t="s">
-        <v>197</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="R34" s="4"/>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.4">
+        <v>191</v>
+      </c>
+      <c r="M34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2681,32 +2768,27 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>157</v>
+        <v>28</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>158</v>
+        <v>43</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H35" t="s">
-        <v>202</v>
-      </c>
-      <c r="I35" t="s">
-        <v>203</v>
-      </c>
-      <c r="J35" t="s">
-        <v>204</v>
-      </c>
-      <c r="R35" s="4"/>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="H35"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="4"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2714,52 +2796,46 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>147</v>
+        <v>45</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="P36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>20</v>
-      </c>
-      <c r="R36" t="s">
-        <v>56</v>
-      </c>
-      <c r="S36" t="s">
-        <v>57</v>
-      </c>
-      <c r="T36" t="s">
-        <v>58</v>
-      </c>
-      <c r="U36" t="s">
-        <v>59</v>
-      </c>
-      <c r="V36" t="s">
-        <v>60</v>
-      </c>
-      <c r="W36" t="s">
-        <v>61</v>
-      </c>
-      <c r="X36" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="H36" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="J36" t="s">
+        <v>193</v>
+      </c>
+      <c r="K36" t="s">
+        <v>194</v>
+      </c>
+      <c r="L36" t="s">
+        <v>195</v>
+      </c>
+      <c r="M36" t="s">
+        <v>196</v>
+      </c>
+      <c r="N36" t="s">
+        <v>197</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -2767,85 +2843,111 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>148</v>
+        <v>52</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="P37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R37" t="s">
         <v>20</v>
       </c>
-      <c r="R37" t="s">
-        <v>56</v>
-      </c>
-      <c r="S37" t="s">
-        <v>57</v>
+      <c r="S37" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="T37" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="U37" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="V37" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="W37" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="X37" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.4">
+        <v>49</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="D38" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>153</v>
+        <v>53</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H38" t="s">
-        <v>202</v>
-      </c>
-      <c r="I38" t="s">
-        <v>203</v>
-      </c>
-      <c r="J38" t="s">
-        <v>204</v>
-      </c>
-      <c r="K38" t="s">
-        <v>205</v>
-      </c>
-      <c r="L38" t="s">
-        <v>206</v>
-      </c>
-      <c r="M38" s="8"/>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="R38" t="s">
+        <v>20</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T38" t="s">
+        <v>34</v>
+      </c>
+      <c r="U38" t="s">
+        <v>46</v>
+      </c>
+      <c r="V38" t="s">
+        <v>47</v>
+      </c>
+      <c r="W38" t="s">
+        <v>48</v>
+      </c>
+      <c r="X38" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>124</v>
       </c>
@@ -2853,21 +2955,302 @@
         <v>150</v>
       </c>
       <c r="C39" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" t="s">
+        <v>193</v>
+      </c>
+      <c r="I39" t="s">
+        <v>194</v>
+      </c>
+      <c r="J39" t="s">
+        <v>195</v>
+      </c>
+      <c r="K39" t="s">
+        <v>196</v>
+      </c>
+      <c r="L39" t="s">
+        <v>197</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="S39" s="4"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H40" t="s">
+        <v>202</v>
+      </c>
+      <c r="I40" t="s">
+        <v>203</v>
+      </c>
+      <c r="J40" t="s">
+        <v>204</v>
+      </c>
+      <c r="S40" s="4"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R41" t="s">
+        <v>20</v>
+      </c>
+      <c r="S41" t="s">
+        <v>56</v>
+      </c>
+      <c r="T41" t="s">
+        <v>57</v>
+      </c>
+      <c r="U41" t="s">
+        <v>58</v>
+      </c>
+      <c r="V41" t="s">
+        <v>59</v>
+      </c>
+      <c r="W41" t="s">
+        <v>60</v>
+      </c>
+      <c r="X41" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" t="s">
         <v>123</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="R42" t="s">
+        <v>20</v>
+      </c>
+      <c r="S42" t="s">
+        <v>56</v>
+      </c>
+      <c r="T42" t="s">
+        <v>57</v>
+      </c>
+      <c r="U42" t="s">
+        <v>58</v>
+      </c>
+      <c r="V42" t="s">
+        <v>59</v>
+      </c>
+      <c r="W42" t="s">
+        <v>60</v>
+      </c>
+      <c r="X42" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H43" t="s">
+        <v>202</v>
+      </c>
+      <c r="I43" t="s">
+        <v>203</v>
+      </c>
+      <c r="J43" t="s">
+        <v>204</v>
+      </c>
+      <c r="K43" t="s">
+        <v>205</v>
+      </c>
+      <c r="L43" t="s">
+        <v>206</v>
+      </c>
+      <c r="M43" s="8"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
         <v>154</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G39" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="H39" s="8"/>
+      <c r="G44" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" t="s">
+        <v>245</v>
+      </c>
+      <c r="C45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" t="s">
+        <v>245</v>
+      </c>
+      <c r="C46" t="s">
+        <v>249</v>
+      </c>
+      <c r="D46" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" t="s">
+        <v>245</v>
+      </c>
+      <c r="C47" t="s">
+        <v>252</v>
+      </c>
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="G47" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
modify documents/api명세서, finished group by consumer_gender, consumer_age, sales_date(hour) in sales_consumer.
</commit_message>
<xml_diff>
--- a/documents/API 명세서.xlsx
+++ b/documents/API 명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\TJSManager_main\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED38A41-84DE-4B6A-820E-CECF0111E6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B5A1A2-3A5B-4382-B871-90D5CDBA73B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="279">
   <si>
     <t>시스템</t>
   </si>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3250,7 +3250,9 @@
       <c r="F47" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="G47" s="8"/>
+      <c r="G47" s="8" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
modify documents/api명세서, change getAllSalescConsumerGroupByHour to url.
</commit_message>
<xml_diff>
--- a/documents/API 명세서.xlsx
+++ b/documents/API 명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\TJSManager_main\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B5A1A2-3A5B-4382-B871-90D5CDBA73B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D4021F-68E5-46F1-9B59-CC8D0C775011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -928,10 +928,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/statistics/consumer_hour/all</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>전체 시간대별 판매량</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1033,6 +1029,10 @@
   </si>
   <si>
     <t>wage: int(시급)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/hour/all</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1535,7 +1535,7 @@
         <v>236</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>157</v>
@@ -1550,7 +1550,7 @@
         <v>208</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>240</v>
@@ -1572,7 +1572,7 @@
         <v>236</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>157</v>
@@ -1605,7 +1605,7 @@
         <v>236</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>128</v>
@@ -1629,16 +1629,16 @@
         <v>236</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>157</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>260</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>261</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>208</v>
@@ -1650,28 +1650,28 @@
         <v>240</v>
       </c>
       <c r="J5" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="L5" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="N5" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="O5" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="P5" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="Q5" s="16" t="s">
         <v>277</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.4">
@@ -1682,16 +1682,16 @@
         <v>236</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>262</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>263</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>208</v>
@@ -1706,16 +1706,16 @@
         <v>236</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>265</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>266</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>208</v>
@@ -1730,16 +1730,16 @@
         <v>236</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>151</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>208</v>
@@ -1751,28 +1751,28 @@
         <v>240</v>
       </c>
       <c r="J8" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="K8" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="L8" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="M8" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="N8" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="N8" s="16" t="s">
+      <c r="O8" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="P8" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="Q8" s="16" t="s">
         <v>277</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>278</v>
       </c>
       <c r="R8" s="4"/>
     </row>
@@ -1784,16 +1784,16 @@
         <v>236</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>154</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>208</v>
@@ -3239,16 +3239,16 @@
         <v>245</v>
       </c>
       <c r="C47" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="D47" t="s">
         <v>128</v>
       </c>
       <c r="E47" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>253</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>208</v>

</xml_diff>

<commit_message>
create statistics API, add documents/api명세서 and api_json_samples.
</commit_message>
<xml_diff>
--- a/documents/API 명세서.xlsx
+++ b/documents/API 명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\TJSManager_main\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D4021F-68E5-46F1-9B59-CC8D0C775011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BBBE77-5137-4EC6-B8D7-C44BFCDE01F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="288">
   <si>
     <t>시스템</t>
   </si>
@@ -769,10 +769,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>매점 정보 생성</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>createManagedStore</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -781,10 +777,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>모든 매점 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>getAllManagedStore</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -797,22 +789,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>한 매점 정보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>매점 정보 수정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>updateManagedStore</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>매점 정보 삭제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>deleteManagedStore</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -913,9 +893,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>getAllSalesConsumerGroupByGender</t>
-  </si>
-  <si>
     <t>/statistics/consumer_age/all</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -924,18 +901,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>getAllSalesConsumerGroupByAge</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>전체 시간대별 판매량</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>getAllSalesConsumerGroupByHour</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>empNum: Long(직원 번호)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1032,7 +1001,75 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/statistics/hour/all</t>
+    <t>지점 정보 생성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 지점 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 지점 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지점 정보 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지점 정보 삭제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupByConsumerGender</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupByConsumerAge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/sales_hour/all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getAllSalesConsumerGroupBySalesHour</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/consumer_gender/one_item/{find_item_num}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 물품에 대한 성별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getOneItemGroupByConsumerGender</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/consumer_age/one_item/{find_item_num}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 물품에 대한 나이대별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getOneItemGroupByConsumerAge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/statistics/sales_hour/one_item/{find_item_num}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 물품에 대한 시간대별 판매량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getOneItemGroupBySalesHour</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1454,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD47"/>
+  <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1529,31 +1566,31 @@
     </row>
     <row r="2" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>157</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>208</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
@@ -1566,22 +1603,22 @@
     </row>
     <row r="3" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>157</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>208</v>
@@ -1599,22 +1636,22 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>208</v>
@@ -1623,22 +1660,22 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A5" s="16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>157</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>208</v>
@@ -1647,51 +1684,51 @@
         <v>187</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>208</v>
@@ -1700,22 +1737,22 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A7" s="16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>128</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>208</v>
@@ -1724,22 +1761,22 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>151</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>208</v>
@@ -1748,52 +1785,52 @@
         <v>187</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="Q8" s="16" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A9" s="16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>154</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>208</v>
@@ -2103,25 +2140,25 @@
         <v>157</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>213</v>
-      </c>
       <c r="G18" s="8" t="s">
         <v>208</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="R18" s="4"/>
     </row>
@@ -2139,13 +2176,13 @@
         <v>128</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>215</v>
+        <v>271</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H19"/>
       <c r="R19" s="4"/>
@@ -2158,19 +2195,19 @@
         <v>210</v>
       </c>
       <c r="C20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D20" t="s">
         <v>128</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>219</v>
+        <v>272</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H20"/>
       <c r="N20" s="6"/>
@@ -2184,31 +2221,31 @@
         <v>210</v>
       </c>
       <c r="C21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D21" t="s">
         <v>151</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>226</v>
-      </c>
       <c r="K21" s="8" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -2221,19 +2258,19 @@
         <v>210</v>
       </c>
       <c r="C22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D22" t="s">
         <v>154</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>222</v>
+        <v>274</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H22"/>
       <c r="N22" s="4"/>
@@ -2253,13 +2290,13 @@
         <v>10</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>109</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>178</v>
@@ -2289,13 +2326,13 @@
         <v>128</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>129</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I24" s="4"/>
       <c r="R24" s="4" t="s">
@@ -2334,13 +2371,13 @@
         <v>128</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>138</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I25" s="4"/>
       <c r="R25" s="4"/>
@@ -2374,10 +2411,10 @@
         <v>151</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>208</v>
@@ -2559,10 +2596,10 @@
         <v>151</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>208</v>
@@ -2811,7 +2848,7 @@
         <v>208</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>187</v>
@@ -3190,19 +3227,19 @@
         <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C45" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D45" t="s">
         <v>128</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>208</v>
@@ -3213,19 +3250,19 @@
         <v>124</v>
       </c>
       <c r="B46" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C46" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D46" t="s">
         <v>128</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>208</v>
@@ -3236,21 +3273,90 @@
         <v>124</v>
       </c>
       <c r="B47" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D47" t="s">
         <v>128</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>253</v>
+        <v>278</v>
       </c>
       <c r="G47" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C48" t="s">
+        <v>279</v>
+      </c>
+      <c r="D48" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" t="s">
+        <v>240</v>
+      </c>
+      <c r="C49" t="s">
+        <v>282</v>
+      </c>
+      <c r="D49" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" t="s">
+        <v>240</v>
+      </c>
+      <c r="C50" t="s">
+        <v>285</v>
+      </c>
+      <c r="D50" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>208</v>
       </c>
     </row>

</xml_diff>